<commit_message>
print tiprates to excel
</commit_message>
<xml_diff>
--- a/output/total_20200801_20200815.xlsx
+++ b/output/total_20200801_20200815.xlsx
@@ -727,8 +727,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="9" width="9.7109375" style="1" customWidth="1"/>
+    <col min="1" max="3" width="11" style="1" customWidth="1"/>
+    <col min="4" max="9" width="9.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="22.5" customHeight="1">

</xml_diff>